<commit_message>
Test senaryoları ve bug raporları eklendi.
</commit_message>
<xml_diff>
--- a/test-senaryoları/TestSenaryoları.xlsx
+++ b/test-senaryoları/TestSenaryoları.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilkin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilkin\Desktop\petstore-api-proje\test-senaryoları\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69672BF7-2269-4944-A01D-0B25FC109B09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B9E2CD-A5D5-4AB7-82D8-83FF5D617EC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="149">
   <si>
     <t>ID</t>
   </si>
@@ -203,18 +203,6 @@
   <si>
     <t xml:space="preserve">Şifre alanına karakter girişi yapılır.
 </t>
-  </si>
-  <si>
-    <t>C29</t>
-  </si>
-  <si>
-    <t>Geçersiz eposta ile kayıt olma kontrolü</t>
-  </si>
-  <si>
-    <t>Ad, soyad alanı doldurulur.
-Eposta alanı geçersiz eposta ile doldurulur.
-Şifre alanı doldurulur.
-Gönder butonuna tıklanır.</t>
   </si>
   <si>
     <t>C16</t>
@@ -628,16 +616,7 @@
 Şimdi öde butonuna tıklanır.</t>
   </si>
   <si>
-    <t>Hatalı giriş mesajı görüntülenmemiştir.
-Geçersiz eposta ile başarıyla giriş yapıldığı görülmüştür. (BUG)</t>
-  </si>
-  <si>
     <t>Preconditions</t>
-  </si>
-  <si>
-    <t>Geçersiz eposta kullanılır. 
-"jsnjhs@kjnfjd.com"
- "dfjbfdjhv"</t>
   </si>
   <si>
     <t>Eposta alanı doldurulmamalıdır.</t>
@@ -943,7 +922,7 @@
       <charset val="162"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -986,12 +965,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1005,7 +978,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1054,9 +1027,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1075,10 +1045,13 @@
     <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1087,11 +1060,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1615,13 +1585,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>67235</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>44824</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>3801035</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>1121149</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2095,10 +2065,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O29"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="G16" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2106,7 +2076,7 @@
     <col min="1" max="1" width="9.140625" style="10"/>
     <col min="2" max="2" width="75.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="88.28515625" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="88.28515625" style="20" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="124.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
     <col min="8" max="8" width="112.5703125" bestFit="1" customWidth="1"/>
@@ -2129,8 +2099,8 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22" t="s">
-        <v>120</v>
+      <c r="D1" s="21" t="s">
+        <v>116</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>3</v>
@@ -2176,8 +2146,8 @@
       <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="20" t="s">
-        <v>131</v>
+      <c r="D2" s="19" t="s">
+        <v>126</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="14" t="s">
@@ -2188,13 +2158,13 @@
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="13" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>18</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>18</v>
@@ -2219,8 +2189,8 @@
       <c r="C3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="20" t="s">
-        <v>132</v>
+      <c r="D3" s="19" t="s">
+        <v>127</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="16" t="s">
@@ -2231,13 +2201,13 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="J3" s="1">
         <v>1</v>
       </c>
       <c r="K3" s="13" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="L3" s="1">
         <v>1</v>
@@ -2262,11 +2232,11 @@
       <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="19" t="s">
-        <v>122</v>
+      <c r="D4" s="18" t="s">
+        <v>117</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F4" s="16" t="s">
         <v>22</v>
@@ -2297,11 +2267,11 @@
       <c r="C5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="19" t="s">
-        <v>123</v>
+      <c r="D5" s="18" t="s">
+        <v>118</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F5" s="16" t="s">
         <v>22</v>
@@ -2333,7 +2303,7 @@
         <v>15</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>22</v>
@@ -2365,7 +2335,7 @@
         <v>15</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F7" s="16" t="s">
         <v>22</v>
@@ -2388,16 +2358,16 @@
     </row>
     <row r="8" spans="1:15" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="23" t="s">
-        <v>144</v>
+      <c r="E8" s="22" t="s">
+        <v>139</v>
       </c>
       <c r="F8" s="14" t="s">
         <v>16</v>
@@ -2405,8 +2375,8 @@
       <c r="G8" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="23" t="s">
-        <v>145</v>
+      <c r="H8" s="22" t="s">
+        <v>140</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -2420,30 +2390,30 @@
     </row>
     <row r="9" spans="1:15" ht="243.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="29" t="s">
-        <v>152</v>
+      <c r="E9" s="24" t="s">
+        <v>147</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="30" t="s">
-        <v>153</v>
+      <c r="H9" s="25" t="s">
+        <v>148</v>
       </c>
       <c r="I9" s="13"/>
       <c r="J9" s="1"/>
-      <c r="K9" s="29" t="s">
-        <v>152</v>
+      <c r="K9" s="24" t="s">
+        <v>147</v>
       </c>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
@@ -2454,15 +2424,15 @@
     </row>
     <row r="10" spans="1:15" ht="243.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="23"/>
+      <c r="E10" s="22"/>
       <c r="F10" s="16" t="s">
         <v>22</v>
       </c>
@@ -2471,7 +2441,7 @@
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="13" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -2492,11 +2462,11 @@
       <c r="C11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="19" t="s">
-        <v>124</v>
+      <c r="D11" s="18" t="s">
+        <v>119</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F11" s="14" t="s">
         <v>16</v>
@@ -2527,8 +2497,8 @@
       <c r="C12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="20" t="s">
-        <v>133</v>
+      <c r="D12" s="19" t="s">
+        <v>128</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>42</v>
@@ -2571,13 +2541,13 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="13" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>18</v>
       </c>
       <c r="K13" s="13" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>18</v>
@@ -2586,7 +2556,7 @@
         <v>18</v>
       </c>
       <c r="N13" s="13" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>15</v>
@@ -2611,13 +2581,13 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="13" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>48</v>
       </c>
       <c r="K14" s="13" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>48</v>
@@ -2626,7 +2596,7 @@
         <v>48</v>
       </c>
       <c r="N14" s="13" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="O14" s="1" t="s">
         <v>15</v>
@@ -2671,7 +2641,7 @@
         <v>15</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F16" s="16" t="s">
         <v>22</v>
@@ -2692,7 +2662,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>54</v>
       </c>
@@ -2702,57 +2672,65 @@
       <c r="C17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="E17" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="H17" s="2" t="s">
+      <c r="E17" s="1"/>
+      <c r="F17" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
+      <c r="G17" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="H17" s="1"/>
+      <c r="I17" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K17" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N17" s="13" t="s">
+        <v>107</v>
+      </c>
       <c r="O17" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" s="15" t="s">
         <v>57</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="G18" s="15" t="s">
-        <v>60</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="13" t="s">
-        <v>90</v>
+        <v>130</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>48</v>
       </c>
       <c r="K18" s="13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>48</v>
@@ -2761,287 +2739,287 @@
         <v>48</v>
       </c>
       <c r="N18" s="13" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="O18" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="228.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="C19" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>125</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="16" t="s">
         <v>22</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="13" t="s">
-        <v>135</v>
+        <v>86</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="K19" s="13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="N19" s="13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O19" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="228.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="322.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="C20" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>121</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="16" t="s">
         <v>22</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="K20" s="13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="N20" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="O20" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="322.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="E21" s="1"/>
-      <c r="F21" s="16" t="s">
-        <v>22</v>
+      <c r="C21" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="E21" s="26"/>
+      <c r="F21" s="29" t="s">
+        <v>56</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="H21" s="1"/>
-      <c r="I21" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="J21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H21" s="26"/>
+      <c r="I21" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="J21" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="K21" s="13" t="s">
+      <c r="K21" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="L21" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="M21" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="N21" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="O21" s="26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="179.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="9"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="26"/>
+      <c r="M22" s="26"/>
+      <c r="N22" s="27"/>
+      <c r="O22" s="26"/>
+    </row>
+    <row r="23" spans="1:15" ht="408.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="E23" s="26"/>
+      <c r="F23" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="G23" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="H23" s="26"/>
+      <c r="I23" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="J23" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="K23" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="L23" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="M23" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="N23" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="O23" s="26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="9"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="26"/>
+      <c r="K24" s="27"/>
+      <c r="L24" s="26"/>
+      <c r="M24" s="26"/>
+      <c r="N24" s="27"/>
+      <c r="O24" s="26"/>
+    </row>
+    <row r="25" spans="1:15" ht="223.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="F25" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="H25" s="1"/>
+      <c r="I25" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K25" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="L21" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="N21" s="13" t="s">
+      <c r="L25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N25" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="O21" s="1" t="s">
+      <c r="O25" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="B22" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="C22" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="28" t="s">
-        <v>127</v>
-      </c>
-      <c r="E22" s="25"/>
-      <c r="F22" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="G22" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="H22" s="25"/>
-      <c r="I22" s="27" t="s">
+    <row r="26" spans="1:15" ht="197.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="E26" s="1"/>
+      <c r="F26" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" s="23" t="s">
         <v>141</v>
-      </c>
-      <c r="J22" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="K22" s="27" t="s">
-        <v>102</v>
-      </c>
-      <c r="L22" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="M22" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="N22" s="27" t="s">
-        <v>114</v>
-      </c>
-      <c r="O22" s="25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" ht="179.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="9"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="27"/>
-      <c r="J23" s="25"/>
-      <c r="K23" s="27"/>
-      <c r="L23" s="25"/>
-      <c r="M23" s="25"/>
-      <c r="N23" s="27"/>
-      <c r="O23" s="25"/>
-    </row>
-    <row r="24" spans="1:15" ht="408.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="B24" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="C24" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24" s="28" t="s">
-        <v>127</v>
-      </c>
-      <c r="E24" s="25"/>
-      <c r="F24" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="G24" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="H24" s="25"/>
-      <c r="I24" s="27" t="s">
-        <v>140</v>
-      </c>
-      <c r="J24" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="K24" s="27" t="s">
-        <v>103</v>
-      </c>
-      <c r="L24" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="M24" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="N24" s="27" t="s">
-        <v>115</v>
-      </c>
-      <c r="O24" s="25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="27"/>
-      <c r="J25" s="25"/>
-      <c r="K25" s="27"/>
-      <c r="L25" s="25"/>
-      <c r="M25" s="25"/>
-      <c r="N25" s="27"/>
-      <c r="O25" s="25"/>
-    </row>
-    <row r="26" spans="1:15" ht="223.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D26" s="19" t="s">
-        <v>128</v>
-      </c>
-      <c r="E26" s="1"/>
-      <c r="F26" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="G26" s="15" t="s">
-        <v>60</v>
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="13" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>48</v>
       </c>
       <c r="K26" s="13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>48</v>
@@ -3049,14 +3027,14 @@
       <c r="M26" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="N26" s="13" t="s">
-        <v>116</v>
+      <c r="N26" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="O26" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="197.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" ht="195" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>75</v>
       </c>
@@ -3066,68 +3044,68 @@
       <c r="C27" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D27" s="19" t="s">
-        <v>129</v>
+      <c r="D27" s="18" t="s">
+        <v>125</v>
       </c>
       <c r="E27" s="1"/>
-      <c r="F27" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="G27" s="24" t="s">
-        <v>146</v>
+      <c r="F27" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" s="23" t="s">
+        <v>141</v>
       </c>
       <c r="H27" s="1"/>
       <c r="I27" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>48</v>
+        <v>131</v>
+      </c>
+      <c r="J27" s="1">
+        <v>1</v>
       </c>
       <c r="K27" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="L27" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="M27" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="N27" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="L27" s="1">
+        <v>1</v>
+      </c>
+      <c r="M27" s="1">
+        <v>1</v>
+      </c>
+      <c r="N27" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="144" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="O27" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" ht="195" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
+      <c r="B28" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="C28" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D28" s="19" t="s">
-        <v>130</v>
+      <c r="D28" s="18" t="s">
+        <v>125</v>
       </c>
       <c r="E28" s="1"/>
-      <c r="F28" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="G28" s="24" t="s">
-        <v>146</v>
+      <c r="F28" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28" s="23" t="s">
+        <v>141</v>
       </c>
       <c r="H28" s="1"/>
       <c r="I28" s="13" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="J28" s="1">
         <v>1</v>
       </c>
-      <c r="K28" s="13" t="s">
-        <v>106</v>
+      <c r="K28" s="7" t="s">
+        <v>104</v>
       </c>
       <c r="L28" s="1">
         <v>1</v>
@@ -3136,84 +3114,41 @@
         <v>1</v>
       </c>
       <c r="N28" s="13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" ht="144" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D29" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="E29" s="1"/>
-      <c r="F29" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="G29" s="24" t="s">
-        <v>146</v>
-      </c>
-      <c r="H29" s="1"/>
-      <c r="I29" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="J29" s="1">
-        <v>1</v>
-      </c>
-      <c r="K29" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="L29" s="1">
-        <v>1</v>
-      </c>
-      <c r="M29" s="1">
-        <v>1</v>
-      </c>
-      <c r="N29" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="O29" s="1" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="26">
-    <mergeCell ref="O22:O23"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="O24:O25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="K24:K25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="L24:L25"/>
-    <mergeCell ref="M24:M25"/>
-    <mergeCell ref="N24:N25"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="M22:M23"/>
-    <mergeCell ref="N22:N23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="L23:L24"/>
+    <mergeCell ref="M23:M24"/>
+    <mergeCell ref="N23:N24"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="K21:K22"/>
+    <mergeCell ref="L21:L22"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="N21:N22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="O23:O24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="K23:K24"/>
+    <mergeCell ref="O21:O22"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="D21:D22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>